<commit_message>
1) Array -> Fifth Question -> Chocolate Distribution Problem -> Approach1 Implemented 3) DSA Sheet Updated
</commit_message>
<xml_diff>
--- a/src/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/src/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PA40084335/Documents/ParryApplications/IntelliJ_Practice/DSASheetPractice/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BB2C85-653D-4B4A-99BB-E8FAC323BCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790198C-E31A-BB4F-A9E9-92C4A06AB49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="500" windowWidth="34880" windowHeight="10020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2831,8 +2831,8 @@
   </sheetPr>
   <dimension ref="A1:AB919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3383,7 +3383,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="39"/>
+      <c r="F16" s="42"/>
       <c r="G16">
         <v>5</v>
       </c>

</xml_diff>